<commit_message>
Tested functionality with added company case
</commit_message>
<xml_diff>
--- a/Blizzard Database.xlsx
+++ b/Blizzard Database.xlsx
@@ -8,21 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helen\Desktop\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5406263-0752-4293-A2D2-A55EE9CBCA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB9218A-97D1-49F5-9188-41F97BDC730B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Take-Two" sheetId="1" r:id="rId2"/>
-    <sheet name="EA" sheetId="3" r:id="rId3"/>
+    <sheet name="Take-Two" sheetId="1" r:id="rId1"/>
+    <sheet name="EA" sheetId="3" r:id="rId2"/>
+    <sheet name="Konami" sheetId="6" r:id="rId3"/>
     <sheet name="Graphs Practise" sheetId="4" r:id="rId4"/>
-    <sheet name="Graphs Automation" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Time</t>
   </si>
@@ -113,13 +109,13 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Sum of Price</t>
-  </si>
-  <si>
     <t>EA</t>
   </si>
   <si>
     <t>Take-Two</t>
+  </si>
+  <si>
+    <t>Konami</t>
   </si>
 </sst>
 </file>
@@ -171,11 +167,10 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -187,9 +182,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
@@ -213,6 +214,9 @@
       <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
@@ -229,191 +233,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[Blizzard Database.xlsx]Sheet1!PivotTable1</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Price</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:delete val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>577.09</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BFDF-4793-9C52-AD190EA39E2C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1650629935"/>
-        <c:axId val="1652406095"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1650629935"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1652406095"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1652406095"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1650629935"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1546,47 +1365,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>86360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E3194D4-EE7E-4F4D-84D3-D8330120F17E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1622,135 +1400,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Helena Szwedzinski" refreshedDate="44018.484449537034" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="4" xr:uid="{E734A755-D403-4421-BC83-3FF5DC370FF5}">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Table1"/>
-  </cacheSource>
-  <cacheFields count="8">
-    <cacheField name="Time" numFmtId="169">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T09:00:00" maxDate="1900-01-11T12:00:00"/>
-    </cacheField>
-    <cacheField name="Open" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="142.78" maxValue="145.03"/>
-    </cacheField>
-    <cacheField name="High" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="145.32" maxValue="147.36000000000001"/>
-    </cacheField>
-    <cacheField name="Low" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="141.69" maxValue="143.69"/>
-    </cacheField>
-    <cacheField name="Close" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="143.68" maxValue="145.36000000000001"/>
-    </cacheField>
-    <cacheField name="Price" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="142.63999999999999" maxValue="145.03"/>
-    </cacheField>
-    <cacheField name="Change" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.0400000000000205" maxValue="0.62999999999999545"/>
-    </cacheField>
-    <cacheField name="Change(%)" numFmtId="10">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-7.2383073496660663E-3" maxValue="4.362880886426561E-3"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="4">
-  <r>
-    <d v="1899-12-30T09:00:00"/>
-    <n v="145.01"/>
-    <n v="146.08500000000001"/>
-    <n v="143.51"/>
-    <n v="144.11000000000001"/>
-    <n v="144.4"/>
-    <n v="0.28999999999999998"/>
-    <n v="2.0119999999999999E-3"/>
-  </r>
-  <r>
-    <d v="1899-12-30T10:00:00"/>
-    <n v="143.97999999999999"/>
-    <n v="145.32"/>
-    <n v="142.87"/>
-    <n v="144.4"/>
-    <n v="145.03"/>
-    <n v="0.62999999999999545"/>
-    <n v="4.362880886426561E-3"/>
-  </r>
-  <r>
-    <d v="1899-12-30T11:00:00"/>
-    <n v="145.03"/>
-    <n v="146.32"/>
-    <n v="141.69"/>
-    <n v="143.68"/>
-    <n v="142.63999999999999"/>
-    <n v="-1.0400000000000205"/>
-    <n v="-7.2383073496660663E-3"/>
-  </r>
-  <r>
-    <d v="1900-01-11T12:00:00"/>
-    <n v="142.78"/>
-    <n v="147.36000000000001"/>
-    <n v="143.69"/>
-    <n v="145.36000000000001"/>
-    <n v="145.02000000000001"/>
-    <n v="-0.34000000000000341"/>
-    <n v="-2.3445042063163935E-3"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6E870086-12AF-46ED-86D5-0F02FEF7F78F}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:A4" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="8">
-    <pivotField numFmtId="169" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="10" showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Price" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2295,7 +1944,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A6119E6-B23E-4C80-BEE9-4BC7238A954C}" name="Table1" displayName="Table1" ref="A3:H13" totalsRowShown="0">
   <autoFilter ref="A3:H13" xr:uid="{1783DA17-7E39-422F-A7E8-C76B5C7234EE}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{65199EA5-2F94-4E5C-A430-F360A0DEE8F6}" name="Time" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{65199EA5-2F94-4E5C-A430-F360A0DEE8F6}" name="Time" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{3E6A8139-32BF-47E2-ABDC-1741E030BEBB}" name="Open"/>
     <tableColumn id="3" xr3:uid="{E4A9FEAE-3C42-4630-BAE4-C800033C4D13}" name="High"/>
     <tableColumn id="4" xr3:uid="{9489CB91-D070-4973-8CFC-E50D9036D5B4}" name="Low"/>
@@ -2304,7 +1953,7 @@
     <tableColumn id="7" xr3:uid="{75340749-5369-40A5-A0C3-1DD92160F635}" name="Change">
       <calculatedColumnFormula>F4-E4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{99735B99-0428-4F0B-9621-7A3E9AE5310E}" name="Change(%)" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{99735B99-0428-4F0B-9621-7A3E9AE5310E}" name="Change(%)" dataDxfId="10">
       <calculatedColumnFormula>G4/E4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2316,14 +1965,35 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA014A02-A460-4D01-8BD9-0D43323E2A52}" name="Table2" displayName="Table2" ref="A3:H7" totalsRowShown="0">
   <autoFilter ref="A3:H7" xr:uid="{BE734998-FB14-4001-8373-3C4541CC022B}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A239CF1F-4151-4AE7-A140-0CD623E41278}" name="Time" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{51F0EB09-9143-4BF1-A90E-86C6D91D090D}" name="Open" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{681D4B33-371C-4812-BDB2-3FB17DCABD12}" name="High" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A663DED2-45C1-4BED-AE8D-5D177E6AF8BA}" name="Low" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5CFA4983-9930-4BF1-90A7-9E798836A19C}" name="Close" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{FE77CF95-3183-424B-8FBD-35583E467CBE}" name="Price" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{FCC882CE-F03C-443F-8488-834F1A914CD5}" name="Change" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A239CF1F-4151-4AE7-A140-0CD623E41278}" name="Time" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{51F0EB09-9143-4BF1-A90E-86C6D91D090D}" name="Open" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{681D4B33-371C-4812-BDB2-3FB17DCABD12}" name="High" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A663DED2-45C1-4BED-AE8D-5D177E6AF8BA}" name="Low" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{5CFA4983-9930-4BF1-90A7-9E798836A19C}" name="Close" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{FE77CF95-3183-424B-8FBD-35583E467CBE}" name="Price" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{FCC882CE-F03C-443F-8488-834F1A914CD5}" name="Change" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{2D5868EE-1377-41BD-A968-AD60E183EAD7}" name="Change(%)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{250EF0DF-50A8-42B0-B3DE-5A882B4E71F0}" name="Table3" displayName="Table3" ref="A3:H13" totalsRowShown="0">
+  <autoFilter ref="A3:H13" xr:uid="{BB6522E7-9297-485F-ACDE-9D61BC78B1E0}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{4FA31D57-50F1-406E-9682-040E1759AB93}" name="Time" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{CC1EAEFE-3633-4E61-AEF2-E30BAB22856F}" name="Open"/>
+    <tableColumn id="3" xr3:uid="{FB22571E-FAB5-4BE2-A335-5FC2E9549E3D}" name="High"/>
+    <tableColumn id="4" xr3:uid="{4C5E0149-3E55-4490-B6C4-FD4A7081753B}" name="Low"/>
+    <tableColumn id="5" xr3:uid="{57BC89CF-A246-4A8C-ABCC-75C0700FD8AB}" name="Close"/>
+    <tableColumn id="6" xr3:uid="{9E2C1670-D68C-4AED-88A9-F50E3CA592F9}" name="Price"/>
+    <tableColumn id="7" xr3:uid="{716937EB-6D0D-45BE-8FFA-8208BE838421}" name="Change" dataDxfId="1">
+      <calculatedColumnFormula>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{D3163F48-6EF8-48C0-AFF1-013BF214C142}" name="Change(%)" dataDxfId="0">
+      <calculatedColumnFormula>G4/E4</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2591,41 +2261,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C3FF97-7844-4D9D-98A1-F07449FB152D}">
-  <dimension ref="A3:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>577.09</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2636,7 +2275,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2671,7 +2310,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>0.375</v>
       </c>
       <c r="B4" s="1" cm="1">
@@ -2704,54 +2343,54 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>0.41666666666666669</v>
       </c>
       <c r="B5" s="1">
         <v>145.01</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>145.32</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>142.87</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>145.03</v>
       </c>
-      <c r="G5" s="5">
-        <f>F5-E5</f>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G13" si="1">F5-E5</f>
         <v>0.91999999999998749</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" si="0"/>
         <v>6.3840122128928419E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>0.45833333333333331</v>
       </c>
       <c r="B6" s="1">
         <v>145.01</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>146.32</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>141.69</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>142.63999999999999</v>
       </c>
-      <c r="G6" s="5">
-        <f>F6-E6</f>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
         <v>-1.4700000000000273</v>
       </c>
       <c r="H6" s="2">
@@ -2760,26 +2399,26 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>12.5</v>
       </c>
       <c r="B7" s="1">
         <v>145.01</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>147.36000000000001</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>143.69</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>145.02000000000001</v>
       </c>
-      <c r="G7" s="5">
-        <f>F7-E7</f>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
         <v>0.90999999999999659</v>
       </c>
       <c r="H7" s="2">
@@ -2788,26 +2427,26 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>145.01</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>148.44</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>142.36000000000001</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>148.36000000000001</v>
       </c>
-      <c r="G8" s="5">
-        <f>F8-E8</f>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
       <c r="H8" s="2">
@@ -2816,26 +2455,26 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>145.01</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>149.26</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>141.26</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>145.36000000000001</v>
       </c>
-      <c r="G9" s="5">
-        <f>F9-E9</f>
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
       <c r="H9" s="2">
@@ -2844,55 +2483,55 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>0.625</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>145.01</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>147.36000000000001</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>143.33000000000001</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>145.55000000000001</v>
       </c>
-      <c r="G10" s="5">
-        <f>F10-E10</f>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
         <v>1.4399999999999977</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>9.9923669419193506E-3</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>145.01</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>145.29</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>143.87</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>143.87</v>
       </c>
-      <c r="G11" s="5">
-        <f>F11-E11</f>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
         <v>-0.24000000000000909</v>
       </c>
       <c r="H11" s="2">
@@ -2901,26 +2540,26 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>145.01</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>148.36000000000001</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>142.96</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>144.51</v>
       </c>
-      <c r="G12" s="5">
-        <f>F12-E12</f>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
         <v>0.39999999999997726</v>
       </c>
       <c r="H12" s="2">
@@ -2929,31 +2568,204 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>0.75</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>145.01</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>147.26</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>143.56</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>144.11000000000001</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>144.38999999999999</v>
       </c>
-      <c r="G13" s="5">
-        <f>F13-E13</f>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
         <v>0.27999999999997272</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="0"/>
         <v>1.942960238706354E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0827C7CE-D9F0-4FA2-A0CC-B23952823C15}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="9.21875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="B4" s="4" cm="1">
+        <f t="array" ref="B4">_FV(A2,"Open")</f>
+        <v>136.41999999999999</v>
+      </c>
+      <c r="C4" s="4" cm="1">
+        <f t="array" ref="C4">_FV(A2,"High")</f>
+        <v>136.41999999999999</v>
+      </c>
+      <c r="D4" s="4" cm="1">
+        <f t="array" ref="D4">_FV(A2,"Low")</f>
+        <v>133.47</v>
+      </c>
+      <c r="E4" s="4" cm="1">
+        <f t="array" ref="E4">_FV(A2,"Previous close",TRUE)</f>
+        <v>135.22</v>
+      </c>
+      <c r="F4" s="4" cm="1">
+        <f t="array" ref="F4">_FV(A2,"Price")</f>
+        <v>133.84</v>
+      </c>
+      <c r="G4" s="4" cm="1">
+        <f t="array" ref="G4">_FV(A2,"Change")</f>
+        <v>-1.38</v>
+      </c>
+      <c r="H4" s="2" cm="1">
+        <f t="array" ref="H4">_FV(A2,"Change (%)",TRUE)</f>
+        <v>-1.0206E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B5" s="4">
+        <v>137.26</v>
+      </c>
+      <c r="C5" s="4">
+        <v>138.63999999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>132.69</v>
+      </c>
+      <c r="E5" s="4">
+        <v>134.88999999999999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>135.74</v>
+      </c>
+      <c r="G5" s="4">
+        <f>Table2[[#This Row],[Price]]-Table2[[#This Row],[Close]]</f>
+        <v>0.85000000000002274</v>
+      </c>
+      <c r="H5" s="7">
+        <f>Table2[[#This Row],[Change]]/Table2[[#This Row],[Close]]</f>
+        <v>6.3014307954631392E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>11.458333333333334</v>
+      </c>
+      <c r="B6" s="4">
+        <v>135.78</v>
+      </c>
+      <c r="C6" s="4">
+        <v>140.36000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>134.66999999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>136.88999999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>137.22</v>
+      </c>
+      <c r="G6" s="4">
+        <f>Table2[[#This Row],[Price]]-Table2[[#This Row],[Close]]</f>
+        <v>0.33000000000001251</v>
+      </c>
+      <c r="H6" s="7">
+        <f>Table2[[#This Row],[Change]]/Table2[[#This Row],[Close]]</f>
+        <v>2.4106947183871177E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>136.25</v>
+      </c>
+      <c r="C7" s="4">
+        <v>144.35</v>
+      </c>
+      <c r="D7" s="4">
+        <v>135.47</v>
+      </c>
+      <c r="E7" s="4">
+        <v>137.33000000000001</v>
+      </c>
+      <c r="F7" s="4">
+        <v>136.97999999999999</v>
+      </c>
+      <c r="G7" s="4">
+        <f>Table2[[#This Row],[Price]]-Table2[[#This Row],[Close]]</f>
+        <v>-0.35000000000002274</v>
+      </c>
+      <c r="H7" s="2">
+        <f>Table2[[#This Row],[Change]]/Table2[[#This Row],[Close]]</f>
+        <v>-2.5486055486785312E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2965,27 +2777,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0827C7CE-D9F0-4FA2-A0CC-B23952823C15}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3B2066-F5BC-4730-97B0-887873606D95}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="7" max="7" width="9.21875" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="e" vm="2">
-        <v>#VALUE!</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -3015,120 +2818,283 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>0.375</v>
       </c>
-      <c r="B4" s="5" cm="1">
-        <f t="array" ref="B4">_FV(A2,"Open")</f>
-        <v>136.41999999999999</v>
-      </c>
-      <c r="C4" s="5" cm="1">
-        <f t="array" ref="C4">_FV(A2,"High")</f>
-        <v>136.41999999999999</v>
-      </c>
-      <c r="D4" s="5" cm="1">
-        <f t="array" ref="D4">_FV(A2,"Low")</f>
-        <v>133.47</v>
-      </c>
-      <c r="E4" s="5" cm="1">
-        <f t="array" ref="E4">_FV(A2,"Previous close",TRUE)</f>
-        <v>135.22</v>
-      </c>
-      <c r="F4" s="5" cm="1">
-        <f t="array" ref="F4">_FV(A2,"Price")</f>
-        <v>133.84</v>
-      </c>
-      <c r="G4" s="5" cm="1">
-        <f t="array" ref="G4">_FV(A2,"Change")</f>
-        <v>-1.38</v>
-      </c>
-      <c r="H4" s="2" cm="1">
-        <f t="array" ref="H4">_FV(A2,"Change (%)",TRUE)</f>
-        <v>-1.0206E-2</v>
+      <c r="B4" s="1">
+        <v>96.36</v>
+      </c>
+      <c r="C4" s="1">
+        <v>98.23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>90.64</v>
+      </c>
+      <c r="E4" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F4" s="1">
+        <v>98.01</v>
+      </c>
+      <c r="G4" s="1">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>6.3200000000000074</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H13" si="0">G4/E4</f>
+        <v>6.8927909259461309E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B5" s="5">
-        <v>137.26</v>
-      </c>
-      <c r="C5" s="5">
-        <v>138.63999999999999</v>
-      </c>
-      <c r="D5" s="5">
-        <v>132.69</v>
-      </c>
-      <c r="E5" s="5">
-        <v>134.88999999999999</v>
-      </c>
-      <c r="F5" s="5">
-        <v>135.74</v>
-      </c>
-      <c r="G5" s="5">
-        <f>Table2[[#This Row],[Price]]-Table2[[#This Row],[Close]]</f>
-        <v>0.85000000000002274</v>
-      </c>
-      <c r="H5" s="8">
-        <f>Table2[[#This Row],[Change]]/Table2[[#This Row],[Close]]</f>
-        <v>6.3014307954631392E-3</v>
+      <c r="B5" s="1">
+        <v>96.36</v>
+      </c>
+      <c r="C5" s="4">
+        <v>97.25</v>
+      </c>
+      <c r="D5" s="4">
+        <v>89.36</v>
+      </c>
+      <c r="E5" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F5" s="4">
+        <v>95.64</v>
+      </c>
+      <c r="G5" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>3.9500000000000028</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="0"/>
+        <v>4.3079943287163303E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>11.458333333333334</v>
-      </c>
-      <c r="B6" s="5">
-        <v>135.78</v>
-      </c>
-      <c r="C6" s="5">
-        <v>140.36000000000001</v>
-      </c>
-      <c r="D6" s="5">
-        <v>134.66999999999999</v>
-      </c>
-      <c r="E6" s="5">
-        <v>136.88999999999999</v>
-      </c>
-      <c r="F6" s="5">
-        <v>137.22</v>
-      </c>
-      <c r="G6" s="5">
-        <f>Table2[[#This Row],[Price]]-Table2[[#This Row],[Close]]</f>
-        <v>0.33000000000001251</v>
-      </c>
-      <c r="H6" s="8">
-        <f>Table2[[#This Row],[Change]]/Table2[[#This Row],[Close]]</f>
-        <v>2.4106947183871177E-3</v>
+      <c r="A6" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B6" s="1">
+        <v>96.36</v>
+      </c>
+      <c r="C6" s="4">
+        <v>98.16</v>
+      </c>
+      <c r="D6" s="4">
+        <v>90.54</v>
+      </c>
+      <c r="E6" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F6" s="4">
+        <v>94.78</v>
+      </c>
+      <c r="G6" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>3.0900000000000034</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.3700512596793582E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="5">
-        <v>136.25</v>
-      </c>
-      <c r="C7" s="5">
-        <v>144.35</v>
-      </c>
-      <c r="D7" s="5">
-        <v>135.47</v>
-      </c>
-      <c r="E7" s="5">
-        <v>137.33000000000001</v>
-      </c>
-      <c r="F7" s="5">
-        <v>136.97999999999999</v>
-      </c>
-      <c r="G7" s="5">
-        <f>Table2[[#This Row],[Price]]-Table2[[#This Row],[Close]]</f>
-        <v>-0.35000000000002274</v>
+      <c r="A7" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>96.36</v>
+      </c>
+      <c r="C7" s="4">
+        <v>98.03</v>
+      </c>
+      <c r="D7" s="4">
+        <v>91.03</v>
+      </c>
+      <c r="E7" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F7" s="4">
+        <v>95.16</v>
+      </c>
+      <c r="G7" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>3.4699999999999989</v>
       </c>
       <c r="H7" s="2">
-        <f>Table2[[#This Row],[Change]]/Table2[[#This Row],[Close]]</f>
-        <v>-2.5486055486785312E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.7844912204166199E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B8" s="4">
+        <v>96.36</v>
+      </c>
+      <c r="C8" s="4">
+        <v>97.49</v>
+      </c>
+      <c r="D8" s="4">
+        <v>90.64</v>
+      </c>
+      <c r="E8" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F8" s="4">
+        <v>94.99</v>
+      </c>
+      <c r="G8" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>3.2999999999999972</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5990838695604724E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B9" s="4">
+        <v>96.36</v>
+      </c>
+      <c r="C9" s="4">
+        <v>97.34</v>
+      </c>
+      <c r="D9" s="4">
+        <v>90.88</v>
+      </c>
+      <c r="E9" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F9" s="4">
+        <v>95.48</v>
+      </c>
+      <c r="G9" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>3.7900000000000063</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1334932926164317E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="B10" s="4">
+        <v>96.36</v>
+      </c>
+      <c r="C10" s="4">
+        <v>97.82</v>
+      </c>
+      <c r="D10" s="4">
+        <v>90.47</v>
+      </c>
+      <c r="E10" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F10" s="4">
+        <v>95</v>
+      </c>
+      <c r="G10" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>3.3100000000000023</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>3.609990184316722E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B11" s="4">
+        <v>96.36</v>
+      </c>
+      <c r="C11" s="4">
+        <v>98.16</v>
+      </c>
+      <c r="D11" s="4">
+        <v>89.23</v>
+      </c>
+      <c r="E11" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F11" s="4">
+        <v>94.36</v>
+      </c>
+      <c r="G11" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>2.6700000000000017</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.9119860399171138E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B12" s="4">
+        <v>96.36</v>
+      </c>
+      <c r="C12" s="4">
+        <v>98.17</v>
+      </c>
+      <c r="D12" s="4">
+        <v>87.29</v>
+      </c>
+      <c r="E12" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F12" s="4">
+        <v>95.79</v>
+      </c>
+      <c r="G12" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>4.1000000000000085</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4715890500599945E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="B13" s="4">
+        <v>96.36</v>
+      </c>
+      <c r="C13" s="4">
+        <v>96.98</v>
+      </c>
+      <c r="D13" s="4">
+        <v>91.01</v>
+      </c>
+      <c r="E13" s="1">
+        <v>91.69</v>
+      </c>
+      <c r="F13" s="4">
+        <v>96.24</v>
+      </c>
+      <c r="G13" s="4">
+        <f>Table3[[#This Row],[Price]]-Table3[[#This Row],[Close]]</f>
+        <v>4.5499999999999972</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9623732140909559E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3152,18 +3118,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF62A12C-08CD-4B3F-8069-7E281A840111}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>